<commit_message>
Update hotel data in Excel file This commit reflects changes in hotel data stored in the Excel file to provide up-to-date information for the application.
</commit_message>
<xml_diff>
--- a/src/Hotels/Example/Hotels Example.xlsx
+++ b/src/Hotels/Example/Hotels Example.xlsx
@@ -5,15 +5,16 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dkatson/Library/CloudStorage/GoogleDrive-dmitry.katson@gmail.com/My Drive/Katson.com Pte. Ltd./Marketing/MVP Activities/Blogs/Function Calling/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Shared/Function-Calling-Copilot/src/Hotels/Example/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB538B99-B541-D349-B91D-9181FCE065F8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E40895F2-7E14-164E-95A4-496E0D8DA6FE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4340" yWindow="500" windowWidth="20120" windowHeight="15940" xr2:uid="{B5630671-2649-7B4F-98A6-89096DC2A665}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet3" sheetId="3" r:id="rId1"/>
+    <sheet name="Hotels" sheetId="3" r:id="rId1"/>
+    <sheet name="Reservations" sheetId="4" r:id="rId2"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="99">
   <si>
     <t>Code</t>
   </si>
@@ -309,6 +310,30 @@
   </si>
   <si>
     <t>3.70</t>
+  </si>
+  <si>
+    <t>Reservation Code</t>
+  </si>
+  <si>
+    <t>Hotel Code</t>
+  </si>
+  <si>
+    <t>Customer Name</t>
+  </si>
+  <si>
+    <t>Check-In Date</t>
+  </si>
+  <si>
+    <t>Check-Out Date</t>
+  </si>
+  <si>
+    <t>Number of Rooms</t>
+  </si>
+  <si>
+    <t>J02</t>
+  </si>
+  <si>
+    <t>Adatum Corporation</t>
   </si>
 </sst>
 </file>
@@ -344,9 +369,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1021,4 +1047,67 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BF8462B6-56ED-5646-B1AE-18CA85FD42E3}">
+  <dimension ref="A1:F2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="15.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="20.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.83203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.33203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.33203125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>91</v>
+      </c>
+      <c r="B1" t="s">
+        <v>92</v>
+      </c>
+      <c r="C1" t="s">
+        <v>93</v>
+      </c>
+      <c r="D1" t="s">
+        <v>94</v>
+      </c>
+      <c r="E1" t="s">
+        <v>95</v>
+      </c>
+      <c r="F1" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>97</v>
+      </c>
+      <c r="B2" t="s">
+        <v>30</v>
+      </c>
+      <c r="C2" t="s">
+        <v>98</v>
+      </c>
+      <c r="D2" s="2">
+        <v>45510</v>
+      </c>
+      <c r="E2" s="2">
+        <v>45602</v>
+      </c>
+      <c r="F2">
+        <v>2</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>